<commit_message>
before swtich fuel and area
</commit_message>
<xml_diff>
--- a/data/scenario_and_base_data/_EXCELFILES/base_data_fuel.xlsx
+++ b/data/scenario_and_base_data/_EXCELFILES/base_data_fuel.xlsx
@@ -9,17 +9,20 @@
   <sheets>
     <sheet name="base_data_fuel" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>REGION_NR</t>
   </si>
   <si>
     <t>ED_ELEC_APPLIANCES</t>
+  </si>
+  <si>
+    <t>GAS_HEATING</t>
   </si>
 </sst>
 </file>
@@ -952,6 +955,53 @@
             </a:rPr>
             <a:t>https://www.iea.org/statistics/resources/unitconverter/</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>23231 --&gt; 270176.530 GWh</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1247,27 +1297,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1275,8 +1329,12 @@
         <f xml:space="preserve"> 82805.6*4.893964</f>
         <v>405247.62539840007</v>
       </c>
+      <c r="C2">
+        <f>270176.53*0.893964</f>
+        <v>241528.09146492003</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1284,8 +1342,12 @@
         <f xml:space="preserve"> 82805.6*8.646003</f>
         <v>715937.46601680003</v>
       </c>
+      <c r="C3">
+        <f xml:space="preserve"> 270176.53*8.646003</f>
+        <v>2335947.0889095902</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1293,6 +1355,10 @@
         <f xml:space="preserve"> 82805.6*86.46003</f>
         <v>7159374.6601680005</v>
       </c>
+      <c r="C4">
+        <f xml:space="preserve"> 270176.53*86.46003</f>
+        <v>23359470.889095902</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>